<commit_message>
Update with skip connection
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/knoor_deakin_edu_au/Documents/Deep Learning with Python/Google_Drive/Projects/Deep Learning/HD-CapsNet/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:40009_{94317FCF-2B78-4027-9398-BA13ECD0880C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{467C7F4A-9211-47A9-A0BB-5AC00319A905}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:40009_{94317FCF-2B78-4027-9398-BA13ECD0880C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C02EBF82-B786-43B0-8E96-BED5C588359E}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="74">
   <si>
     <t>Dataset</t>
   </si>
@@ -264,12 +264,27 @@
   </si>
   <si>
     <t>Decreasing primary capsule  worked without the loss</t>
+  </si>
+  <si>
+    <t>Mod-2.7</t>
+  </si>
+  <si>
+    <t>Mod-2.8</t>
+  </si>
+  <si>
+    <t>Mod-3.1</t>
+  </si>
+  <si>
+    <t>Mod-3.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#.00,,"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -762,7 +777,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -780,6 +795,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -825,7 +841,447 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="66">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1360,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17:Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1827,7 @@
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1411,8 +1867,20 @@
       <c r="M1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1452,8 +1920,20 @@
       <c r="M2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1493,8 +1973,20 @@
       <c r="M3">
         <v>4.84</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="7">
+        <v>4857920</v>
+      </c>
+      <c r="O3" s="7">
+        <v>4857920</v>
+      </c>
+      <c r="P3" s="7">
+        <v>5229632</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>5229632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1534,8 +2026,20 @@
       <c r="M4" s="2">
         <v>0.98670000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="2">
+        <v>0.98680001497268599</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.98790001869201605</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.98710000514984098</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1575,8 +2079,20 @@
       <c r="M5" s="2">
         <v>0.9274</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="2">
+        <v>0.93580001592636097</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.92110002040863004</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.94279998540878296</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0.94010001420974698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1616,8 +2132,20 @@
       <c r="M6" s="2">
         <v>0.89449999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="2">
+        <v>0.90770000219345004</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.88669997453689497</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.91219997406005804</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.90969997644424405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1657,8 +2185,20 @@
       <c r="M7" s="2">
         <v>0.93579999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="2">
+        <v>0.94316666666666604</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.93027166666666605</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.94735333333333305</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0.94533833333333295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1698,8 +2238,20 @@
       <c r="M8" s="2">
         <v>0.93740000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="2">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0.94893333333333296</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0.94730000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1739,8 +2291,20 @@
       <c r="M9" s="2">
         <v>0.93640000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="2">
+        <v>0.94368095238095195</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0.93124523809523796</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0.94800833333333301</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0.946154761904761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1780,8 +2344,20 @@
       <c r="M10" s="2">
         <v>0.99099999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.98839999999999995</v>
+      </c>
+      <c r="P10" s="2">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0.9899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1821,8 +2397,20 @@
       <c r="M11" s="2">
         <v>0.89159999999999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="2">
+        <v>0.90549999999999997</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.88170000000000004</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0.90949999999999998</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0.90580000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1862,8 +2450,20 @@
       <c r="M14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1903,8 +2503,20 @@
       <c r="M15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" t="s">
+        <v>71</v>
+      </c>
+      <c r="P15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1938,8 +2550,20 @@
       <c r="K16">
         <v>5.55</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N16" s="7">
+        <v>6104384</v>
+      </c>
+      <c r="O16" s="7">
+        <v>6104384</v>
+      </c>
+      <c r="P16" s="7">
+        <v>7845184</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>7845184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1973,8 +2597,20 @@
       <c r="K17" s="2">
         <v>0.86780000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N17" s="2">
+        <v>0.861500024795532</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.85360002517700195</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0.86930000782012895</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0.86809998750686601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2008,8 +2644,20 @@
       <c r="K18" s="2">
         <v>0.78879999999999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N18" s="2">
+        <v>0.774500012397766</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.76630002260208097</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0.79309999942779497</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0.78729999065399103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2043,8 +2691,20 @@
       <c r="K19" s="2">
         <v>0.56859999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N19" s="2">
+        <v>0.61180001497268599</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.60070002079009999</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0.66380000114440896</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0.66229999065399103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2078,8 +2738,20 @@
       <c r="K20" s="2">
         <v>0.73970000000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N20" s="2">
+        <v>0.74747999999999903</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0.73819666666666595</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0.77425166666666601</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>0.77838166666666597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2113,8 +2785,20 @@
       <c r="K21" s="2">
         <v>0.754</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N21" s="2">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0.75376666666666603</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0.79196666666666604</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>0.79559999999999897</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2148,8 +2832,20 @@
       <c r="K22" s="2">
         <v>0.74519999999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N22" s="2">
+        <v>0.75331111111111104</v>
+      </c>
+      <c r="O22" s="2">
+        <v>0.74424444444444404</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0.78118968253968202</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>0.78515198412698395</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2183,8 +2879,20 @@
       <c r="K23" s="2">
         <v>0.9103</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N23" s="2">
+        <v>0.90680000000000005</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0.89859999999999995</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0.89780000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2218,107 +2926,22 @@
       <c r="K24" s="2">
         <v>0.55679999999999996</v>
       </c>
+      <c r="N24" s="2">
+        <v>0.59519999999999995</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0.58509999999999995</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>0.64410000000000001</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B6:M6">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="greaterThan">
-      <formula>$B$6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="30" operator="greaterThan">
-      <formula>$B$6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:M4">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="greaterThan">
-      <formula>$B$4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="29" operator="greaterThan">
-      <formula>$B$4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:M5">
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="greaterThan">
-      <formula>$B$5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="greaterThan">
-      <formula>$B$5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:M7">
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="greaterThan">
-      <formula>$B$7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:M8">
-    <cfRule type="cellIs" dxfId="14" priority="26" operator="greaterThan">
-      <formula>$B$8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:M9">
-    <cfRule type="cellIs" dxfId="13" priority="25" operator="greaterThan">
-      <formula>$B$9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10:M10">
-    <cfRule type="cellIs" dxfId="12" priority="24" operator="greaterThan">
-      <formula>$B$10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:M11">
-    <cfRule type="cellIs" dxfId="11" priority="23" operator="greaterThan">
-      <formula>$B$11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:K16">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
-      <formula>$B$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:K17">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="greaterThan">
-      <formula>$B$17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:K18">
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="greaterThan">
-      <formula>$B$18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:K19">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
-      <formula>$B$19</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="16" operator="greaterThan">
-      <formula>$B$19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:K20">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="greaterThan">
-      <formula>$B$20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:K21">
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="greaterThan">
-      <formula>$B$21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22:K22">
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="greaterThan">
-      <formula>$B$22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23:K23">
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="greaterThan">
-      <formula>$B$23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:K24">
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="greaterThan">
-      <formula>$B$24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:M4">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="B3:Q3">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2329,7 +2952,103 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:M5">
+  <conditionalFormatting sqref="B4:Q4">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:Q5">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:Q6">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:Q7">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:Q8">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:Q9">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:Q10">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:Q11">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:Q17">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2341,7 +3060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:M6">
+  <conditionalFormatting sqref="B18:Q18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2353,7 +3072,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:M7">
+  <conditionalFormatting sqref="B19:Q19">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2365,10 +3084,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:M8">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
-      <formula>$H$8</formula>
+  <conditionalFormatting sqref="B20:Q20">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:Q21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2380,7 +3108,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:M9">
+  <conditionalFormatting sqref="B22:Q22">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2392,7 +3120,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10:M10">
+  <conditionalFormatting sqref="B23:Q23">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2404,7 +3132,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:M11">
+  <conditionalFormatting sqref="B24:Q24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2425,9 +3153,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2E2853-D516-48B7-9C6C-D2BAE28B57DC}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J2" sqref="J2"/>
+      <selection pane="topRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update with results for Top down approach with skip connections
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/knoor_deakin_edu_au/Documents/Deep Learning with Python/Google_Drive/Projects/Deep Learning/HD-CapsNet/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="13_ncr:40009_{94317FCF-2B78-4027-9398-BA13ECD0880C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A043F01F-A255-4BAF-A805-75EBF8991AA2}"/>
+  <xr:revisionPtr revIDLastSave="364" documentId="13_ncr:40009_{94317FCF-2B78-4027-9398-BA13ECD0880C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{270EFFD4-D006-4795-A6AD-B341C2C104BD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
-    <sheet name="Analysis CIFAR_10" sheetId="2" r:id="rId2"/>
-    <sheet name="Analysis CIFAR_100" sheetId="3" r:id="rId3"/>
+    <sheet name="Result_Summary" sheetId="4" r:id="rId2"/>
+    <sheet name="Analysis CIFAR_10" sheetId="2" r:id="rId3"/>
+    <sheet name="Analysis CIFAR_100" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="90">
   <si>
     <t>Dataset</t>
   </si>
@@ -111,9 +112,6 @@
   <si>
     <t>Total  Trainable 
 params (M)</t>
-  </si>
-  <si>
-    <t>Total  Trainable &lt;br /&gt;params (M)</t>
   </si>
   <si>
     <t>Analysis</t>
@@ -293,6 +291,47 @@
   </si>
   <si>
     <t>Increasing Secondary capsule dimension  improved the performance</t>
+  </si>
+  <si>
+    <t>Total  Trainable
+params (M)</t>
+  </si>
+  <si>
+    <t>Mod-3.3</t>
+  </si>
+  <si>
+    <t>Mod-3.4</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>HD-CapsNet (W/O Lc)</t>
+  </si>
+  <si>
+    <t>HD-CapsNet
+(W/O Lc)</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Primary Capsule Dimention</t>
+  </si>
+  <si>
+    <t>Secondary Capsule Dimention
+(Coarse)</t>
+  </si>
+  <si>
+    <t>Secondary Capsule Dimention
+(Medium)</t>
+  </si>
+  <si>
+    <t>Secondary Capsule Dimention
+(Fine)</t>
+  </si>
+  <si>
+    <t>Loss Function</t>
   </si>
 </sst>
 </file>
@@ -302,7 +341,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#.00,,"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +472,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -794,7 +839,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -813,6 +858,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1172,18 +1226,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="18" max="19" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1235,8 +1292,14 @@
       <c r="Q1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1277,21 +1340,27 @@
         <v>14</v>
       </c>
       <c r="N2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" t="s">
         <v>70</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>71</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>5.04</v>
@@ -1341,8 +1410,14 @@
       <c r="Q3" s="7">
         <v>5229632</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="7">
+        <v>5802304</v>
+      </c>
+      <c r="S3" s="7">
+        <v>5802304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1394,8 +1469,14 @@
       <c r="Q4" s="2">
         <v>0.98710000514984098</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="2">
+        <v>0.98820000886917103</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.98729997873306197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1447,8 +1528,14 @@
       <c r="Q5" s="2">
         <v>0.94010001420974698</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="2">
+        <v>0.93959999084472601</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.94150000810623102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1500,8 +1587,14 @@
       <c r="Q6" s="2">
         <v>0.90969997644424405</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="2">
+        <v>0.91259998083114602</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.91240000724792403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1553,8 +1646,14 @@
       <c r="Q7" s="2">
         <v>0.94533833333333295</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="2">
+        <v>0.946481666666666</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.94649499999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1606,8 +1705,14 @@
       <c r="Q8" s="2">
         <v>0.94730000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="2">
+        <v>0.94816666666666605</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.94830000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1659,8 +1764,14 @@
       <c r="Q9" s="2">
         <v>0.946154761904761</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="2">
+        <v>0.94719166666666599</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.94725357142857103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1712,8 +1823,14 @@
       <c r="Q10" s="2">
         <v>0.9899</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="2">
+        <v>0.99109999999999998</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.98980000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1765,8 +1882,14 @@
       <c r="Q11" s="2">
         <v>0.90580000000000005</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="2">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.9093</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1818,8 +1941,14 @@
       <c r="Q14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>23</v>
+      </c>
+      <c r="S14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1860,21 +1989,27 @@
         <v>14</v>
       </c>
       <c r="N15" t="s">
+        <v>69</v>
+      </c>
+      <c r="O15" t="s">
         <v>70</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>71</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>72</v>
       </c>
-      <c r="Q15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>79</v>
+      </c>
+      <c r="S15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="B16">
         <v>8.52</v>
@@ -1918,8 +2053,14 @@
       <c r="Q16" s="7">
         <v>7845184</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="7">
+        <v>11676992</v>
+      </c>
+      <c r="S16" s="7">
+        <v>11676992</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1965,8 +2106,14 @@
       <c r="Q17" s="2">
         <v>0.86809998750686601</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="2">
+        <v>0.86949998140335005</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0.872699975967407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2012,8 +2159,14 @@
       <c r="Q18" s="2">
         <v>0.78729999065399103</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="2">
+        <v>0.78759998083114602</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0.79060000181198098</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2059,8 +2212,14 @@
       <c r="Q19" s="2">
         <v>0.66229999065399103</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="2">
+        <v>0.66060000658035201</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0.66610002517700195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2106,8 +2265,14 @@
       <c r="Q20" s="2">
         <v>0.77838166666666597</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="2">
+        <v>0.77074500000000001</v>
+      </c>
+      <c r="S20" s="2">
+        <v>0.773963333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2153,8 +2318,14 @@
       <c r="Q21" s="2">
         <v>0.79559999999999897</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="2">
+        <v>0.78986666666666605</v>
+      </c>
+      <c r="S21" s="2">
+        <v>0.79303333333333303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2200,8 +2371,14 @@
       <c r="Q22" s="2">
         <v>0.78515198412698395</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="2">
+        <v>0.77824126984126896</v>
+      </c>
+      <c r="S22" s="2">
+        <v>0.781436111111111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2247,8 +2424,14 @@
       <c r="Q23" s="2">
         <v>0.89780000000000004</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="2">
+        <v>0.88849999999999996</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0.88849999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2294,8 +2477,15 @@
       <c r="Q24" s="2">
         <v>0.64410000000000001</v>
       </c>
+      <c r="R24" s="2">
+        <v>0.63329999999999997</v>
+      </c>
+      <c r="S24" s="2">
+        <v>0.63929999999999998</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B3:Q3">
     <cfRule type="colorScale" priority="23">
       <colorScale>
@@ -2308,7 +2498,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:Q4">
+  <conditionalFormatting sqref="B4:S4">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -2320,7 +2510,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:Q5">
+  <conditionalFormatting sqref="B5:S5">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2332,7 +2522,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:Q6">
+  <conditionalFormatting sqref="B6:S6">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2344,7 +2534,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:Q7">
+  <conditionalFormatting sqref="B7:S7">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2356,7 +2546,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:Q8">
+  <conditionalFormatting sqref="B8:S8">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -2368,7 +2558,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:Q9">
+  <conditionalFormatting sqref="B9:S9">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2380,7 +2570,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:Q10">
+  <conditionalFormatting sqref="B10:S10">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2392,7 +2582,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:Q11">
+  <conditionalFormatting sqref="B11:S11">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2404,7 +2594,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:Q17">
+  <conditionalFormatting sqref="B17:S17">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2416,7 +2606,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:Q18">
+  <conditionalFormatting sqref="B18:S18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2428,7 +2618,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:Q19">
+  <conditionalFormatting sqref="B19:S19">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2440,7 +2630,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:Q20">
+  <conditionalFormatting sqref="B20:S20">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2452,7 +2642,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:Q21">
+  <conditionalFormatting sqref="B21:S21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2464,7 +2654,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:Q22">
+  <conditionalFormatting sqref="B22:S22">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2476,7 +2666,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:Q23">
+  <conditionalFormatting sqref="B23:S23">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2488,7 +2678,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:Q24">
+  <conditionalFormatting sqref="B24:S24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2506,6 +2696,1331 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E26FB0C-CD72-44F6-B86B-578CAEA29634}">
+  <dimension ref="A2:T39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="10"/>
+    <col min="13" max="13" width="9.7109375" style="10" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="10" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="10" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" style="10" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="10" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="10" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" style="10" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:20" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5.04</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.98809999999999998</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.90990000000000004</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.94469999999999998</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.94630000000000003</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.94530000000000003</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.99080000000000001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4">
+        <v>5.04</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.98719999999999997</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.93810000000000004</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.90839999999999999</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.94410000000000005</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.94589999999999996</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.94479999999999997</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.90559999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5.03</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.98709999999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.93959999999999999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.91159999999999997</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.9456</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.94720000000000004</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.94620000000000004</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.99129999999999996</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.90890000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>4.74</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.98240000000000005</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.91830000000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.87890000000000001</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.92569999999999997</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.92859999999999998</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.92689999999999995</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.98460000000000003</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.87419999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>5.03</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.98809999999999998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.93859999999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.9103</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.94550000000000001</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.9466</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.94589999999999996</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>4.74</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.98619999999999997</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.93010000000000004</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.89670000000000005</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.93730000000000002</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.93940000000000001</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.93820000000000003</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.98950000000000005</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.89280000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>4.84</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.98760000000000003</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.93359999999999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.90259999999999996</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.94089999999999996</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.94179999999999997</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.98939999999999995</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.89849999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>4.84</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.9788</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.89790000000000003</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.85829999999999995</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.91120000000000001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.8528</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>4.84</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.9113</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.87649999999999995</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.92320000000000002</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.9254</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.92410000000000003</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.87250000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>4.84</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.98240000000000005</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.90959999999999996</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.87239999999999995</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.92090000000000005</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.92349999999999999</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.98619999999999997</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.86750000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>4.84</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.98409999999999997</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.91420000000000001</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.87960000000000005</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.92549999999999999</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.92659999999999998</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.98650000000000004</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.87470000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>4.84</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.98670000000000002</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.9274</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.89449999999999996</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.93579999999999997</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.93740000000000001</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.93640000000000001</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.89159999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="7">
+        <v>4857920</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.98680001497268599</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.93580001592636097</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.90770000219345004</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.94316666666666604</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.94368095238095195</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.90549999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="7">
+        <v>4857920</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.92110002040863004</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.88669997453689497</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.93027166666666605</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.93124523809523796</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.98839999999999995</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.88170000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="7">
+        <v>5229632</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.98790001869201605</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.94279998540878296</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.91219997406005804</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.94735333333333305</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.94893333333333296</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.94800833333333301</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.90949999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="7">
+        <v>5229632</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.98710000514984098</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.94010001420974698</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.90969997644424405</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.94533833333333295</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.94730000000000003</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.946154761904761</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.9899</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.90580000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="7">
+        <v>5802304</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.98820000886917103</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.93959999084472601</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.91259998083114602</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.946481666666666</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.94816666666666605</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.94719166666666599</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.99109999999999998</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.90900000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="7">
+        <v>5802304</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.98729997873306197</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.94150000810623102</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.91240000724792403</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.94649499999999998</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.94830000000000003</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.94725357142857103</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.9093</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>8.52</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.86850000000000005</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.66180000000000005</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.77070000000000005</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.78820000000000001</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.90369999999999995</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.64080000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23">
+        <v>8.52</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.86029999999999995</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.77829999999999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.64870000000000005</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.76039999999999996</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.77869999999999995</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.76749999999999996</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.62529999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.86750000000000005</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.78949999999999998</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.66169999999999995</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.7873</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.77680000000000005</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.64039999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>5.22</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.86929999999999996</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.7873</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.75509999999999999</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.76970000000000005</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.76070000000000004</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.90639999999999998</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.60440000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.86180000000000001</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.78310000000000002</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.64690000000000003</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.76139999999999997</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.77980000000000005</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.76859999999999995</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.89829999999999999</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0.62390000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>5.22</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.86450000000000005</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.55179999999999996</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.73119999999999996</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.74260000000000004</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0.73570000000000002</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.9264</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.5393</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>5.55</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.86570000000000003</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.7833</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.57079999999999997</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.73860000000000003</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.74309999999999998</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.92510000000000003</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0.56100000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>5.55</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.874</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.58309999999999995</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.747</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.75980000000000003</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.752</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.91759999999999997</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>5.55</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.86029999999999995</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.77480000000000004</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.57010000000000005</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.73340000000000005</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.74729999999999996</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.73880000000000001</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.55789999999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>5.55</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.86780000000000002</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.78879999999999995</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.56859999999999999</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.73970000000000002</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.754</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.74519999999999997</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.9103</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.55679999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="7">
+        <v>6104384</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.861500024795532</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.774500012397766</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.61180001497268599</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.74747999999999903</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.75331111111111104</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0.90680000000000005</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0.59519999999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="7">
+        <v>6104384</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.85360002517700195</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.76630002260208097</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.60070002079009999</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.73819666666666595</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.75376666666666603</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.74424444444444404</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0.89859999999999995</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0.58509999999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="7">
+        <v>7845184</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.86930000782012895</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.79309999942779497</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.66380000114440896</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.77425166666666601</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.79196666666666604</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.78118968253968202</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="7">
+        <v>7845184</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.86809998750686601</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.78729999065399103</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.66229999065399103</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.77838166666666597</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.79559999999999897</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.78515198412698395</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.89780000000000004</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0.64410000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="7">
+        <v>11676992</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.86949998140335005</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.78759998083114602</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.66060000658035201</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.77074500000000001</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.78986666666666605</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0.77824126984126896</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0.88849999999999996</v>
+      </c>
+      <c r="K38" s="2">
+        <v>0.63329999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="7">
+        <v>11676992</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.872699975967407</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.79060000181198098</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.66610002517700195</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.773963333333333</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.79303333333333303</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0.781436111111111</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0.88849999999999996</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0.63929999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2E2853-D516-48B7-9C6C-D2BAE28B57DC}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
@@ -2521,108 +4036,108 @@
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3248,55 +4763,55 @@
     </row>
     <row r="13" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="L13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3305,11 +4820,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77F9E36-B427-41AC-A8E9-32AE9C4E0B55}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="P13" sqref="P13"/>
     </sheetView>
@@ -3321,108 +4836,108 @@
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="G2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3724,28 +5239,28 @@
     </row>
     <row r="13" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>